<commit_message>
bug fix on the formulas for teams
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -66,121 +66,136 @@
     <t>Team Phi</t>
   </si>
   <si>
+    <t>Legolas Greenleaf</t>
+  </si>
+  <si>
+    <t>Team Mu</t>
+  </si>
+  <si>
+    <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>Team Tau</t>
+  </si>
+  <si>
+    <t>Voldemort</t>
+  </si>
+  <si>
+    <t>Team Chi</t>
+  </si>
+  <si>
+    <t>Pool B</t>
+  </si>
+  <si>
+    <t>Othello</t>
+  </si>
+  <si>
+    <t>Team Omicron</t>
+  </si>
+  <si>
+    <t>Hermione Granger</t>
+  </si>
+  <si>
+    <t>Team Theta</t>
+  </si>
+  <si>
+    <t>Tyrion Lannister</t>
+  </si>
+  <si>
+    <t>Team Upsilon</t>
+  </si>
+  <si>
+    <t>Pool C</t>
+  </si>
+  <si>
+    <t>Frodo Baggins</t>
+  </si>
+  <si>
+    <t>Team Zeta</t>
+  </si>
+  <si>
+    <t>Neville Longbottom</t>
+  </si>
+  <si>
+    <t>Team Xi</t>
+  </si>
+  <si>
+    <t>Ygritte</t>
+  </si>
+  <si>
+    <t>Team Alpha</t>
+  </si>
+  <si>
+    <t>Pool D</t>
+  </si>
+  <si>
+    <t>Petyr Baelish</t>
+  </si>
+  <si>
+    <t>Team Pi</t>
+  </si>
+  <si>
     <t>Quirinus Quirrell</t>
   </si>
   <si>
     <t>Team Rho</t>
   </si>
   <si>
-    <t>Samwise Gamgee</t>
-  </si>
-  <si>
-    <t>Team Tau</t>
-  </si>
-  <si>
-    <t>Ygritte</t>
-  </si>
-  <si>
-    <t>Team Alpha</t>
-  </si>
-  <si>
-    <t>Pool B</t>
-  </si>
-  <si>
     <t>Katniss Everdeen</t>
   </si>
   <si>
     <t>Team Lambda</t>
   </si>
   <si>
+    <t>Pool E</t>
+  </si>
+  <si>
+    <t>Jon Snow</t>
+  </si>
+  <si>
+    <t>Team Kappa</t>
+  </si>
+  <si>
+    <t>Daenerys Targaryen</t>
+  </si>
+  <si>
+    <t>Team Delta</t>
+  </si>
+  <si>
+    <t>Xaro Xhoan Daxos</t>
+  </si>
+  <si>
+    <t>Team Omega</t>
+  </si>
+  <si>
+    <t>Pool F</t>
+  </si>
+  <si>
+    <t>Willy Wonka</t>
+  </si>
+  <si>
+    <t>Team Psi</t>
+  </si>
+  <si>
+    <t>Moby Dick</t>
+  </si>
+  <si>
+    <t>Team Nu</t>
+  </si>
+  <si>
     <t>Ron Weasley</t>
   </si>
   <si>
     <t>Team Sigma</t>
   </si>
   <si>
-    <t>Xaro Xhoan Daxos</t>
-  </si>
-  <si>
-    <t>Team Omega</t>
-  </si>
-  <si>
-    <t>Pool C</t>
-  </si>
-  <si>
-    <t>Willy Wonka</t>
-  </si>
-  <si>
-    <t>Team Psi</t>
-  </si>
-  <si>
-    <t>Moby Dick</t>
-  </si>
-  <si>
-    <t>Team Nu</t>
-  </si>
-  <si>
-    <t>Othello</t>
-  </si>
-  <si>
-    <t>Team Omicron</t>
-  </si>
-  <si>
-    <t>Pool D</t>
-  </si>
-  <si>
-    <t>Hermione Granger</t>
-  </si>
-  <si>
-    <t>Team Theta</t>
-  </si>
-  <si>
-    <t>Jon Snow</t>
-  </si>
-  <si>
-    <t>Team Kappa</t>
-  </si>
-  <si>
-    <t>Tyrion Lannister</t>
-  </si>
-  <si>
-    <t>Team Upsilon</t>
-  </si>
-  <si>
-    <t>Pool E</t>
-  </si>
-  <si>
-    <t>Petyr Baelish</t>
-  </si>
-  <si>
-    <t>Team Pi</t>
-  </si>
-  <si>
-    <t>Legolas Greenleaf</t>
-  </si>
-  <si>
-    <t>Team Mu</t>
-  </si>
-  <si>
-    <t>Daenerys Targaryen</t>
-  </si>
-  <si>
-    <t>Team Delta</t>
-  </si>
-  <si>
-    <t>Pool F</t>
-  </si>
-  <si>
-    <t>Frodo Baggins</t>
-  </si>
-  <si>
-    <t>Team Zeta</t>
-  </si>
-  <si>
-    <t>Neville Longbottom</t>
-  </si>
-  <si>
-    <t>Team Xi</t>
+    <t>Pool G</t>
+  </si>
+  <si>
+    <t>Cersei Lannister</t>
+  </si>
+  <si>
+    <t>Team Gamma</t>
   </si>
   <si>
     <t>Eddard Stark</t>
@@ -189,15 +204,6 @@
     <t>Team Epsilon</t>
   </si>
   <si>
-    <t>Pool G</t>
-  </si>
-  <si>
-    <t>Voldemort</t>
-  </si>
-  <si>
-    <t>Team Chi</t>
-  </si>
-  <si>
     <t>Gandalf The Grey</t>
   </si>
   <si>
@@ -208,12 +214,6 @@
   </si>
   <si>
     <t>Team Iota</t>
-  </si>
-  <si>
-    <t>Cersei Lannister</t>
-  </si>
-  <si>
-    <t>Team Gamma</t>
   </si>
   <si>
     <t>Pool A.1</t>
@@ -5550,7 +5550,7 @@
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25" t="str">
-        <f>CONCATENATE("Pool G.2 ",''!)</f>
+        <f>CONCATENATE("Pool G.2 ",'Pool Matches'!G171)</f>
       </c>
       <c r="I5" s="25" t="str">
         <f>CONCATENATE("Pool C.1 ",'Pool Matches'!G85)</f>
@@ -5561,7 +5561,7 @@
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
       <c r="O5" s="25" t="str">
-        <f>CONCATENATE("Pool F.2 ",''!)</f>
+        <f>CONCATENATE("Pool F.2 ",'Pool Matches'!O123)</f>
       </c>
     </row>
     <row r="6">
@@ -5654,7 +5654,7 @@
         <v>88</v>
       </c>
       <c r="G10" s="25" t="str">
-        <f>CONCATENATE("Pool G.2 ",''!)</f>
+        <f>CONCATENATE("Pool G.2 ",'Pool Matches'!G171)</f>
       </c>
       <c r="I10" s="25" t="str">
         <f>CONCATENATE("Pool C.1 ",'Pool Matches'!G85)</f>
@@ -5673,7 +5673,7 @@
         <v>88</v>
       </c>
       <c r="O10" s="25" t="str">
-        <f>CONCATENATE("Pool F.2 ",''!)</f>
+        <f>CONCATENATE("Pool F.2 ",'Pool Matches'!O123)</f>
       </c>
     </row>
     <row r="11">
@@ -5770,10 +5770,10 @@
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
       <c r="G19" s="25" t="str">
-        <f>CONCATENATE("Pool E.2 ",''!)</f>
+        <f>CONCATENATE("Pool E.2 ",'Pool Matches'!G123)</f>
       </c>
       <c r="I19" s="25" t="str">
-        <f>CONCATENATE("Pool B.2 ",''!)</f>
+        <f>CONCATENATE("Pool B.2 ",'Pool Matches'!O37)</f>
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
@@ -5781,7 +5781,7 @@
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25" t="str">
-        <f>CONCATENATE("Pool A.2 ",''!)</f>
+        <f>CONCATENATE("Pool A.2 ",'Pool Matches'!G48)</f>
       </c>
     </row>
     <row r="20">
@@ -5874,10 +5874,10 @@
         <v>88</v>
       </c>
       <c r="G24" s="25" t="str">
-        <f>CONCATENATE("Pool E.2 ",''!)</f>
+        <f>CONCATENATE("Pool E.2 ",'Pool Matches'!G123)</f>
       </c>
       <c r="I24" s="25" t="str">
-        <f>CONCATENATE("Pool B.2 ",''!)</f>
+        <f>CONCATENATE("Pool B.2 ",'Pool Matches'!O37)</f>
       </c>
       <c r="J24" s="25" t="s">
         <v>88</v>
@@ -5893,7 +5893,7 @@
         <v>88</v>
       </c>
       <c r="O24" s="25" t="str">
-        <f>CONCATENATE("Pool A.2 ",''!)</f>
+        <f>CONCATENATE("Pool A.2 ",'Pool Matches'!G48)</f>
       </c>
     </row>
     <row r="25">
@@ -5990,7 +5990,7 @@
       <c r="E33" s="25"/>
       <c r="F33" s="25"/>
       <c r="G33" s="25" t="str">
-        <f>CONCATENATE("Pool C.2 ",''!)</f>
+        <f>CONCATENATE("Pool C.2 ",'Pool Matches'!G86)</f>
       </c>
       <c r="I33" s="25" t="str">
         <f>CONCATENATE("Pool D.1 ",'Pool Matches'!O85)</f>
@@ -6001,7 +6001,7 @@
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
       <c r="O33" s="25" t="str">
-        <f>CONCATENATE("Pool D.2 ",''!)</f>
+        <f>CONCATENATE("Pool D.2 ",'Pool Matches'!O86)</f>
       </c>
     </row>
     <row r="34">
@@ -6094,7 +6094,7 @@
         <v>88</v>
       </c>
       <c r="G38" s="25" t="str">
-        <f>CONCATENATE("Pool C.2 ",''!)</f>
+        <f>CONCATENATE("Pool C.2 ",'Pool Matches'!G86)</f>
       </c>
       <c r="I38" s="25" t="str">
         <f>CONCATENATE("Pool D.1 ",'Pool Matches'!O85)</f>
@@ -6113,7 +6113,7 @@
         <v>88</v>
       </c>
       <c r="O38" s="25" t="str">
-        <f>CONCATENATE("Pool D.2 ",''!)</f>
+        <f>CONCATENATE("Pool D.2 ",'Pool Matches'!O86)</f>
       </c>
     </row>
     <row r="39">

</xml_diff>